<commit_message>
Memperbarui data dan API Contract
</commit_message>
<xml_diff>
--- a/Data COVID-19 Sulawesi Tengah.xlsx
+++ b/Data COVID-19 Sulawesi Tengah.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17085" windowHeight="12510" firstSheet="1" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17085" windowHeight="12510"/>
   </bookViews>
   <sheets>
     <sheet name="Kasus COVID-19" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
   <si>
     <t>no</t>
   </si>
@@ -144,6 +144,18 @@
   </si>
   <si>
     <t>cluster</t>
+  </si>
+  <si>
+    <t>selesai_pengawasan</t>
+  </si>
+  <si>
+    <t>dalam_pengawasan</t>
+  </si>
+  <si>
+    <t>selesai_pemantauan</t>
+  </si>
+  <si>
+    <t>dalam_pemantauan</t>
   </si>
 </sst>
 </file>
@@ -462,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G14"/>
+  <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -473,7 +485,7 @@
     <col min="2" max="2" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -495,8 +507,20 @@
       <c r="G1" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H1" t="s">
+        <v>39</v>
+      </c>
+      <c r="I1" t="s">
+        <v>40</v>
+      </c>
+      <c r="J1" t="s">
+        <v>41</v>
+      </c>
+      <c r="K1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -518,8 +542,23 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H2">
+        <f t="shared" ref="H2:H13" si="0">F2</f>
+        <v>0</v>
+      </c>
+      <c r="I2">
+        <f t="shared" ref="I2:I13" si="1">D2-F2</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>0</v>
+      </c>
+      <c r="K2">
+        <f>C2</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -541,8 +580,23 @@
       <c r="G3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H3">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I3">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <f t="shared" ref="K3:K14" si="2">C3</f>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -564,8 +618,23 @@
       <c r="G4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H4">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I4">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J4">
+        <v>0</v>
+      </c>
+      <c r="K4">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -587,8 +656,23 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H5">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J5">
+        <v>0</v>
+      </c>
+      <c r="K5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -610,8 +694,23 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H6">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I6">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
+      <c r="K6">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -633,8 +732,23 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H7">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I7">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
+      <c r="K7">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -656,8 +770,23 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H8">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I8">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
+      <c r="K8">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -679,8 +808,23 @@
       <c r="G9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H9">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I9">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J9">
+        <v>0</v>
+      </c>
+      <c r="K9">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -702,8 +846,23 @@
       <c r="G10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I10">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J10">
+        <v>0</v>
+      </c>
+      <c r="K10">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -725,8 +884,23 @@
       <c r="G11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I11">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="J11">
+        <v>0</v>
+      </c>
+      <c r="K11">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -748,8 +922,23 @@
       <c r="G12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H12">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+      <c r="I12">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="J12">
+        <v>0</v>
+      </c>
+      <c r="K12">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -771,8 +960,23 @@
       <c r="G13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="I13">
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+      <c r="J13">
+        <v>0</v>
+      </c>
+      <c r="K13">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -793,6 +997,21 @@
       </c>
       <c r="G14">
         <v>0</v>
+      </c>
+      <c r="H14">
+        <f>F14</f>
+        <v>2</v>
+      </c>
+      <c r="I14">
+        <f>D14-F14</f>
+        <v>4</v>
+      </c>
+      <c r="J14">
+        <v>0</v>
+      </c>
+      <c r="K14">
+        <f t="shared" si="2"/>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -872,7 +1091,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Penambahan data Rumah Sakit dan API contract untuk data rumah sakit
</commit_message>
<xml_diff>
--- a/Data COVID-19 Sulawesi Tengah.xlsx
+++ b/Data COVID-19 Sulawesi Tengah.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="17085" windowHeight="12510"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="17085" windowHeight="12510" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Kasus COVID-19" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <t>no</t>
   </si>
@@ -156,16 +156,106 @@
   </si>
   <si>
     <t>dalam_pemantauan</t>
+  </si>
+  <si>
+    <t>nama_rumah_sakit</t>
+  </si>
+  <si>
+    <t>RSUD Undata Palu</t>
+  </si>
+  <si>
+    <t>RSU Anutapura Palu</t>
+  </si>
+  <si>
+    <t>RSUD Kab. Banggai Luwuk</t>
+  </si>
+  <si>
+    <t>RSU Mokopido Toli-Toli</t>
+  </si>
+  <si>
+    <t>RSUD Kolonedale</t>
+  </si>
+  <si>
+    <t>alamat</t>
+  </si>
+  <si>
+    <t>Jl. R. E. Martadinata, Tondo Kecamatan Mantikulore 94119</t>
+  </si>
+  <si>
+    <t>Jl. Kangkung No. 1 Palu</t>
+  </si>
+  <si>
+    <t>Jl. W Monginsidi 2 Kolonedale</t>
+  </si>
+  <si>
+    <t>Jl. Lanoni No.37 Kel Baru Kec Baolan kab Toli-Toli, Sulteng</t>
+  </si>
+  <si>
+    <t>Jl. Imam Bonjol KM 3 No. 14 Luwuk</t>
+  </si>
+  <si>
+    <t>telepon</t>
+  </si>
+  <si>
+    <t>04514908020</t>
+  </si>
+  <si>
+    <t>0451460570</t>
+  </si>
+  <si>
+    <t>046121820</t>
+  </si>
+  <si>
+    <t>045321301</t>
+  </si>
+  <si>
+    <t>046521010</t>
+  </si>
+  <si>
+    <t>email</t>
+  </si>
+  <si>
+    <t>rsundata@yahoo.com</t>
+  </si>
+  <si>
+    <t>rsu_anutapurapalu@yahoo.com</t>
+  </si>
+  <si>
+    <t>rsud.luwuk@gmail.com</t>
+  </si>
+  <si>
+    <t>mokopido@gmail.com</t>
+  </si>
+  <si>
+    <t>rsudkolonodale@gmail.com</t>
+  </si>
+  <si>
+    <t>longitude</t>
+  </si>
+  <si>
+    <t>latitude</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.00000000"/>
+  </numFmts>
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
@@ -189,13 +279,18 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hipertaut" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -476,7 +571,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
@@ -1077,12 +1172,168 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E13:E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="53" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="11" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="29.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.28515625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>43</v>
+      </c>
+      <c r="C1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E1" t="s">
+        <v>61</v>
+      </c>
+      <c r="F1" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="3">
+        <v>119.88185799999999</v>
+      </c>
+      <c r="G2" s="3">
+        <v>-0.85783860000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C3" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="3">
+        <v>119.84946189999999</v>
+      </c>
+      <c r="G3">
+        <v>-0.8998931</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>46</v>
+      </c>
+      <c r="C4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="F4" s="3">
+        <v>122.8221964</v>
+      </c>
+      <c r="G4" s="3">
+        <v>-0.93409319999999996</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>47</v>
+      </c>
+      <c r="C5" t="s">
+        <v>53</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="F5" s="3">
+        <v>120.82277689999999</v>
+      </c>
+      <c r="G5">
+        <v>1.0358794</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" t="s">
+        <v>48</v>
+      </c>
+      <c r="C6" t="s">
+        <v>52</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="F6" s="3">
+        <v>121.328429</v>
+      </c>
+      <c r="G6" s="3">
+        <v>-1.994421</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E2" r:id="rId1"/>
+    <hyperlink ref="E3" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
+    <hyperlink ref="E5" r:id="rId4"/>
+    <hyperlink ref="E6" r:id="rId5"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>